<commit_message>
aps over xijia update 0630
</commit_message>
<xml_diff>
--- a/03APS/2-测试点xmind&测试用例/APS系统测试用例.xlsx
+++ b/03APS/2-测试点xmind&测试用例/APS系统测试用例.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22365" windowHeight="9300"/>
+    <workbookView windowWidth="28125" windowHeight="12540"/>
   </bookViews>
   <sheets>
     <sheet name="APS系统测试用例" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="196">
   <si>
     <t>功能模块</t>
   </si>
@@ -624,6 +624,173 @@
   </si>
   <si>
     <t>按计划机台数+按最大作业数量+同区域+最少改机+最少改机+高剩余产能优先</t>
+  </si>
+  <si>
+    <t>企划排机</t>
+  </si>
+  <si>
+    <t>aps-042</t>
+  </si>
+  <si>
+    <t>1、用户已登录
+2、数据库连接正常
+5、系统正常</t>
+  </si>
+  <si>
+    <t>1、登录账号进入企划排机页
+2、选择排机日期，点击查询
+3、查看页面返回结果</t>
+  </si>
+  <si>
+    <t>1、账号登录成功
+2、 查询成功</t>
+  </si>
+  <si>
+    <t>aps-044</t>
+  </si>
+  <si>
+    <t>转台查询</t>
+  </si>
+  <si>
+    <t>1、用户已登录
+2、数据库连接正常
+6、系统正常</t>
+  </si>
+  <si>
+    <t>1、登录账号进入企划排机页
+2、选择企划排机状态，点击查询
+3、查看页面返回结果</t>
+  </si>
+  <si>
+    <t>aps-045</t>
+  </si>
+  <si>
+    <t>新增企划排机-保存</t>
+  </si>
+  <si>
+    <t>1、用户已登录
+2、数据库连接正常
+7、系统正常</t>
+  </si>
+  <si>
+    <t>1、登录账号进入企划排机页
+2、点击新增，选择相应数据，点击保存
+3、查看页面返回结果</t>
+  </si>
+  <si>
+    <t>1、账号登录成功
+2、 选择相应数据成功，保存成功
+3、跳转列表页，状态为调整中</t>
+  </si>
+  <si>
+    <t>aps-046</t>
+  </si>
+  <si>
+    <t>新增企划排机--发布</t>
+  </si>
+  <si>
+    <t>1、用户已登录
+2、数据库连接正常
+8、系统正常</t>
+  </si>
+  <si>
+    <t>1、登录账号进入企划排机页
+2、点击新增，选择相应数据，点击发布
+3、查看页面返回结果</t>
+  </si>
+  <si>
+    <t>1、账号登录成功
+2、选择相应数据成功，发布成功
+3、跳转列表页，状态为已发布，原有已发布的状态变更为历史发布</t>
+  </si>
+  <si>
+    <t>aps-047</t>
+  </si>
+  <si>
+    <t>1、用户已登录
+2、数据库连接正常
+9、系统正常</t>
+  </si>
+  <si>
+    <t>1、登录账号进入企划排机页
+2、点击调整，选择相应数据，点击保存
+3、查看页面返回结果</t>
+  </si>
+  <si>
+    <t>1、账号登录成功
+2、 点击调整进入排机页， 保存成功
+3、跳转列表页，状态为调整中</t>
+  </si>
+  <si>
+    <t>aps-048</t>
+  </si>
+  <si>
+    <t>1、用户已登录
+2、数据库连接正常
+10、系统正常</t>
+  </si>
+  <si>
+    <t>1、登录账号进入企划排机页
+2、点击发布
+3、查看页面返回结果</t>
+  </si>
+  <si>
+    <t>1、账号登录成功
+2、 发布成功，状态变为已发布，其他已发布状态变成历史发布</t>
+  </si>
+  <si>
+    <t>aps-049</t>
+  </si>
+  <si>
+    <t>1、用户已登录
+2、数据库连接正常
+11、系统正常</t>
+  </si>
+  <si>
+    <t>1、登录账号进入企划排机页
+2、点击浏览
+3、查看页面返回结果</t>
+  </si>
+  <si>
+    <t>1、账号登录成功
+2、 点击浏览成功，跳转排机详情页</t>
+  </si>
+  <si>
+    <t>aps-050</t>
+  </si>
+  <si>
+    <t>1、用户已登录
+2、数据库连接正常
+12、系统正常</t>
+  </si>
+  <si>
+    <t>1、登录账号进入企划排机页
+2、点击导出
+3、查看页面返回结果</t>
+  </si>
+  <si>
+    <t>1、账号登录成功
+2、 点击导出成功
+3、导出为excel表数据</t>
+  </si>
+  <si>
+    <t>aps-051</t>
+  </si>
+  <si>
+    <t>页面四按时</t>
+  </si>
+  <si>
+    <t>1、用户已登录
+2、数据库连接正常
+13、系统正常</t>
+  </si>
+  <si>
+    <t>1、登录账号进入企划排机页
+2、查看页面返回结果</t>
+  </si>
+  <si>
+    <t>1、账号登录成功
+2、 调整： 状态=已发布和历史发布时， 可用，否则置灰禁用； 点击调整复制一份当前记录并跳转企划排机页面并带出复制的信息， 保存后状态=调整中；修改： 状态=调整中时， 可用， 否则置灰禁用； 点击跳转到企划排机页面， 并带入排序日期，并自动查询；浏览： 默认可用， 跳转到企划排机页面（查询、导出、清空、发布）可用， 其他按钮禁用隐藏；发布： 状态=调整中可用， 否则置灰禁用； 点击修改状态=已发布， 并将当前日期的其他已发布状态=历史发布；导出： 根据企划排机中的导出格式， 导出当前企划排机记录的明细数据。</t>
   </si>
 </sst>
 </file>
@@ -631,10 +798,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -675,29 +842,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="等线"/>
@@ -705,8 +849,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -720,37 +872,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F76"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -764,9 +893,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -788,26 +917,10 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="等线"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -820,9 +933,63 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="等线"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -847,7 +1014,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -859,7 +1092,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -871,7 +1116,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -883,37 +1128,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -925,109 +1188,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1070,30 +1237,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -1119,21 +1262,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -1152,6 +1280,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1166,153 +1303,183 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="21" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1702,9 +1869,9 @@
   <dimension ref="A1:Y146"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomLeft" activeCell="I57" sqref="I57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -3433,18 +3600,20 @@
       <c r="X47" s="18"/>
       <c r="Y47" s="18"/>
     </row>
-    <row r="48" spans="1:25">
-      <c r="A48" s="10"/>
-      <c r="B48" s="10"/>
-      <c r="C48" s="10"/>
-      <c r="D48" s="14"/>
-      <c r="E48" s="12"/>
-      <c r="F48" s="13"/>
-      <c r="G48" s="14"/>
-      <c r="H48" s="14"/>
-      <c r="I48" s="19"/>
-      <c r="J48" s="19"/>
-      <c r="K48" s="20"/>
+    <row r="48" ht="18" customHeight="1" spans="1:25">
+      <c r="A48" s="5"/>
+      <c r="B48" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="C48" s="7"/>
+      <c r="D48" s="8"/>
+      <c r="E48" s="8"/>
+      <c r="F48" s="9"/>
+      <c r="G48" s="8"/>
+      <c r="H48" s="8"/>
+      <c r="I48" s="9"/>
+      <c r="J48" s="9"/>
+      <c r="K48" s="5"/>
       <c r="L48" s="18"/>
       <c r="M48" s="18"/>
       <c r="N48" s="18"/>
@@ -3460,15 +3629,25 @@
       <c r="X48" s="18"/>
       <c r="Y48" s="18"/>
     </row>
-    <row r="49" spans="1:25">
+    <row r="49" ht="40.5" spans="1:25">
       <c r="A49" s="10"/>
       <c r="B49" s="10"/>
-      <c r="C49" s="10"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="12"/>
+      <c r="C49" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="D49" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="E49" s="12" t="s">
+        <v>158</v>
+      </c>
       <c r="F49" s="13"/>
-      <c r="G49" s="14"/>
-      <c r="H49" s="14"/>
+      <c r="G49" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="H49" s="12" t="s">
+        <v>160</v>
+      </c>
       <c r="I49" s="19"/>
       <c r="J49" s="19"/>
       <c r="K49" s="20"/>
@@ -3487,15 +3666,25 @@
       <c r="X49" s="18"/>
       <c r="Y49" s="18"/>
     </row>
-    <row r="50" spans="1:25">
+    <row r="50" ht="40.5" spans="1:25">
       <c r="A50" s="10"/>
       <c r="B50" s="10"/>
-      <c r="C50" s="10"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="12"/>
+      <c r="C50" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="D50" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="E50" s="12" t="s">
+        <v>163</v>
+      </c>
       <c r="F50" s="13"/>
-      <c r="G50" s="14"/>
-      <c r="H50" s="14"/>
+      <c r="G50" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="H50" s="12" t="s">
+        <v>160</v>
+      </c>
       <c r="I50" s="19"/>
       <c r="J50" s="19"/>
       <c r="K50" s="20"/>
@@ -3514,15 +3703,25 @@
       <c r="X50" s="18"/>
       <c r="Y50" s="18"/>
     </row>
-    <row r="51" spans="1:25">
+    <row r="51" ht="40.5" spans="1:25">
       <c r="A51" s="10"/>
       <c r="B51" s="10"/>
-      <c r="C51" s="10"/>
-      <c r="D51" s="14"/>
-      <c r="E51" s="12"/>
+      <c r="C51" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="D51" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="E51" s="12" t="s">
+        <v>167</v>
+      </c>
       <c r="F51" s="13"/>
-      <c r="G51" s="14"/>
-      <c r="H51" s="14"/>
+      <c r="G51" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="H51" s="12" t="s">
+        <v>169</v>
+      </c>
       <c r="I51" s="19"/>
       <c r="J51" s="19"/>
       <c r="K51" s="20"/>
@@ -3541,15 +3740,25 @@
       <c r="X51" s="18"/>
       <c r="Y51" s="18"/>
     </row>
-    <row r="52" spans="1:25">
+    <row r="52" ht="54" spans="1:25">
       <c r="A52" s="10"/>
       <c r="B52" s="10"/>
-      <c r="C52" s="10"/>
-      <c r="D52" s="14"/>
-      <c r="E52" s="12"/>
+      <c r="C52" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="D52" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="E52" s="12" t="s">
+        <v>172</v>
+      </c>
       <c r="F52" s="13"/>
-      <c r="G52" s="14"/>
-      <c r="H52" s="14"/>
+      <c r="G52" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="H52" s="12" t="s">
+        <v>174</v>
+      </c>
       <c r="I52" s="19"/>
       <c r="J52" s="19"/>
       <c r="K52" s="20"/>
@@ -3568,15 +3777,25 @@
       <c r="X52" s="18"/>
       <c r="Y52" s="18"/>
     </row>
-    <row r="53" spans="1:25">
+    <row r="53" ht="40.5" spans="1:25">
       <c r="A53" s="10"/>
       <c r="B53" s="10"/>
-      <c r="C53" s="10"/>
-      <c r="D53" s="14"/>
-      <c r="E53" s="12"/>
+      <c r="C53" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="D53" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="E53" s="12" t="s">
+        <v>176</v>
+      </c>
       <c r="F53" s="13"/>
-      <c r="G53" s="14"/>
-      <c r="H53" s="14"/>
+      <c r="G53" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="H53" s="12" t="s">
+        <v>178</v>
+      </c>
       <c r="I53" s="19"/>
       <c r="J53" s="19"/>
       <c r="K53" s="20"/>
@@ -3595,15 +3814,25 @@
       <c r="X53" s="18"/>
       <c r="Y53" s="18"/>
     </row>
-    <row r="54" spans="1:25">
+    <row r="54" ht="40.5" spans="1:25">
       <c r="A54" s="10"/>
       <c r="B54" s="10"/>
-      <c r="C54" s="10"/>
-      <c r="D54" s="14"/>
-      <c r="E54" s="12"/>
+      <c r="C54" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="D54" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="E54" s="12" t="s">
+        <v>180</v>
+      </c>
       <c r="F54" s="13"/>
-      <c r="G54" s="14"/>
-      <c r="H54" s="14"/>
+      <c r="G54" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="H54" s="12" t="s">
+        <v>182</v>
+      </c>
       <c r="I54" s="19"/>
       <c r="J54" s="19"/>
       <c r="K54" s="20"/>
@@ -3622,15 +3851,25 @@
       <c r="X54" s="18"/>
       <c r="Y54" s="18"/>
     </row>
-    <row r="55" spans="1:25">
+    <row r="55" ht="40.5" spans="1:25">
       <c r="A55" s="10"/>
       <c r="B55" s="10"/>
-      <c r="C55" s="10"/>
-      <c r="D55" s="14"/>
-      <c r="E55" s="12"/>
+      <c r="C55" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="D55" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="E55" s="12" t="s">
+        <v>184</v>
+      </c>
       <c r="F55" s="13"/>
-      <c r="G55" s="14"/>
-      <c r="H55" s="14"/>
+      <c r="G55" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="H55" s="12" t="s">
+        <v>186</v>
+      </c>
       <c r="I55" s="19"/>
       <c r="J55" s="19"/>
       <c r="K55" s="20"/>
@@ -3649,15 +3888,25 @@
       <c r="X55" s="18"/>
       <c r="Y55" s="18"/>
     </row>
-    <row r="56" spans="1:25">
+    <row r="56" ht="40.5" spans="1:25">
       <c r="A56" s="10"/>
       <c r="B56" s="10"/>
-      <c r="C56" s="10"/>
-      <c r="D56" s="14"/>
-      <c r="E56" s="12"/>
+      <c r="C56" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="D56" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="E56" s="12" t="s">
+        <v>188</v>
+      </c>
       <c r="F56" s="13"/>
-      <c r="G56" s="14"/>
-      <c r="H56" s="14"/>
+      <c r="G56" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="H56" s="12" t="s">
+        <v>190</v>
+      </c>
       <c r="I56" s="19"/>
       <c r="J56" s="19"/>
       <c r="K56" s="20"/>
@@ -3676,15 +3925,25 @@
       <c r="X56" s="18"/>
       <c r="Y56" s="18"/>
     </row>
-    <row r="57" spans="1:25">
+    <row r="57" ht="175.5" spans="1:25">
       <c r="A57" s="10"/>
       <c r="B57" s="10"/>
-      <c r="C57" s="10"/>
-      <c r="D57" s="14"/>
-      <c r="E57" s="12"/>
+      <c r="C57" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="D57" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="E57" s="12" t="s">
+        <v>193</v>
+      </c>
       <c r="F57" s="13"/>
-      <c r="G57" s="14"/>
-      <c r="H57" s="14"/>
+      <c r="G57" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="H57" s="12" t="s">
+        <v>195</v>
+      </c>
       <c r="I57" s="19"/>
       <c r="J57" s="19"/>
       <c r="K57" s="20"/>

</xml_diff>